<commit_message>
New input generic file...
</commit_message>
<xml_diff>
--- a/input_generic.xlsx
+++ b/input_generic.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="93">
   <si>
     <t>Description</t>
   </si>
@@ -298,6 +298,15 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Magnetic</t>
+  </si>
+  <si>
+    <t>Throughput Optimized HDD</t>
+  </si>
+  <si>
+    <t>Cold HDD</t>
   </si>
 </sst>
 </file>
@@ -1534,8 +1543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2196,7 +2205,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Help!$I$2:$I$3</xm:f>
+            <xm:f>Help!$I$2:$I$6</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
@@ -2216,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2432,6 +2441,9 @@
       <c r="H4" s="2">
         <v>100</v>
       </c>
+      <c r="I4" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="N4" t="s">
         <v>25</v>
       </c>
@@ -2455,6 +2467,9 @@
       <c r="H5" s="2">
         <v>500</v>
       </c>
+      <c r="I5" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="Q5" t="s">
         <v>30</v>
       </c>
@@ -2474,6 +2489,9 @@
       </c>
       <c r="H6" s="2">
         <v>500</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="S6" s="19" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
Adding amount of instances
</commit_message>
<xml_diff>
--- a/input_generic.xlsx
+++ b/input_generic.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carvaa/Projects/ProposalCalculator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravanini/WorkDocs/workspace/ProposalCalculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180"/>
   </bookViews>
   <sheets>
     <sheet name="Servers" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="93">
   <si>
     <t>Description</t>
   </si>
@@ -459,7 +459,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -487,6 +487,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -505,7 +506,43 @@
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="41">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1215,64 +1252,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q1048576" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
-  <autoFilter ref="A1:Q1048576"/>
-  <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="36"/>
-    <tableColumn id="2" name="Environment" dataDxfId="35"/>
-    <tableColumn id="3" name="Region" dataDxfId="34"/>
-    <tableColumn id="4" name="CPU" dataDxfId="33"/>
-    <tableColumn id="6" name="CPU Tolerance" dataDxfId="32" dataCellStyle="Percent"/>
-    <tableColumn id="17" name="Memory" dataDxfId="31"/>
-    <tableColumn id="7" name="Memory Tolerance" dataDxfId="30" dataCellStyle="Percent"/>
-    <tableColumn id="8" name="Monthly Utilization" dataDxfId="29"/>
-    <tableColumn id="9" name="Storage(GB)" dataDxfId="28"/>
-    <tableColumn id="10" name="Volume Type" dataDxfId="27"/>
-    <tableColumn id="11" name="IOPS" dataDxfId="26"/>
-    <tableColumn id="12" name="Snapshot(GB)" dataDxfId="25"/>
-    <tableColumn id="21" name="S3 Backup(GB)" dataDxfId="24"/>
-    <tableColumn id="18" name="Operating System" dataDxfId="23"/>
-    <tableColumn id="13" name="Only Current Generation Instances" dataDxfId="22"/>
-    <tableColumn id="5" name="Pre Installed S/W" dataDxfId="21"/>
-    <tableColumn id="22" name="Billing Option" dataDxfId="20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:R1048576" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+  <autoFilter ref="A1:R1048576"/>
+  <tableColumns count="18">
+    <tableColumn id="1" name="Description" dataDxfId="38"/>
+    <tableColumn id="14" name="Instances" dataDxfId="1"/>
+    <tableColumn id="2" name="Environment" dataDxfId="37"/>
+    <tableColumn id="3" name="Region" dataDxfId="36"/>
+    <tableColumn id="4" name="CPU" dataDxfId="35"/>
+    <tableColumn id="6" name="CPU Tolerance" dataDxfId="34" dataCellStyle="Percent"/>
+    <tableColumn id="17" name="Memory" dataDxfId="33"/>
+    <tableColumn id="7" name="Memory Tolerance" dataDxfId="32" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="Monthly Utilization" dataDxfId="31"/>
+    <tableColumn id="9" name="Storage(GB)" dataDxfId="30"/>
+    <tableColumn id="10" name="Volume Type" dataDxfId="29"/>
+    <tableColumn id="11" name="IOPS" dataDxfId="28"/>
+    <tableColumn id="12" name="Snapshot(GB)" dataDxfId="27"/>
+    <tableColumn id="21" name="S3 Backup(GB)" dataDxfId="26"/>
+    <tableColumn id="18" name="Operating System" dataDxfId="25"/>
+    <tableColumn id="13" name="Only Current Generation Instances" dataDxfId="24"/>
+    <tableColumn id="5" name="Pre Installed S/W" dataDxfId="23"/>
+    <tableColumn id="22" name="Billing Option" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table4" displayName="Table4" ref="H1:T17" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="H1:T17"/>
-  <tableColumns count="13">
-    <tableColumn id="1" name="Storage(GB)" dataDxfId="17"/>
-    <tableColumn id="2" name="Volume Type" dataDxfId="16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table4" displayName="Table4" ref="H1:U17" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="H1:U17"/>
+  <tableColumns count="14">
+    <tableColumn id="1" name="Storage(GB)" dataDxfId="19"/>
+    <tableColumn id="2" name="Volume Type" dataDxfId="18"/>
     <tableColumn id="3" name="IOPS"/>
-    <tableColumn id="4" name="Snapshot(GB)" dataDxfId="15"/>
-    <tableColumn id="5" name="Term Type" dataDxfId="14"/>
-    <tableColumn id="6" name="Lease Contract Length" dataDxfId="13"/>
+    <tableColumn id="4" name="Snapshot(GB)" dataDxfId="17"/>
+    <tableColumn id="5" name="Term Type" dataDxfId="16"/>
+    <tableColumn id="6" name="Lease Contract Length" dataDxfId="15"/>
     <tableColumn id="7" name="Purchase Option"/>
-    <tableColumn id="8" name="Offering Class" dataDxfId="12"/>
-    <tableColumn id="9" name="Tenancy" dataDxfId="11"/>
+    <tableColumn id="8" name="Offering Class" dataDxfId="14"/>
+    <tableColumn id="9" name="Tenancy" dataDxfId="13"/>
     <tableColumn id="10" name="Operating System"/>
     <tableColumn id="14" name="SAP Instance Type"/>
-    <tableColumn id="11" name="Billing Option" dataDxfId="10"/>
-    <tableColumn id="12" name="Pre Installed S/W" dataDxfId="9"/>
+    <tableColumn id="11" name="Billing Option" dataDxfId="12"/>
+    <tableColumn id="13" name="Only Current Generation Instances" dataDxfId="0"/>
+    <tableColumn id="12" name="Pre Installed S/W" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table5" displayName="Table5" ref="A1:G17" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table5" displayName="Table5" ref="A1:G17" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:G17"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Description" dataDxfId="6"/>
-    <tableColumn id="7" name="Environment" dataDxfId="5"/>
-    <tableColumn id="2" name="Region" dataDxfId="4"/>
-    <tableColumn id="3" name="Instances" dataDxfId="3"/>
-    <tableColumn id="4" name="CPU" dataDxfId="2"/>
-    <tableColumn id="5" name="Monthly Utilization" dataDxfId="1"/>
-    <tableColumn id="6" name="Memory" dataDxfId="0"/>
+    <tableColumn id="1" name="Description" dataDxfId="8"/>
+    <tableColumn id="7" name="Environment" dataDxfId="7"/>
+    <tableColumn id="2" name="Region" dataDxfId="6"/>
+    <tableColumn id="3" name="Instances" dataDxfId="5"/>
+    <tableColumn id="4" name="CPU" dataDxfId="4"/>
+    <tableColumn id="5" name="Monthly Utilization" dataDxfId="3"/>
+    <tableColumn id="6" name="Memory" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1541,622 +1580,656 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" style="15" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="18.5" style="2" customWidth="1"/>
-    <col min="17" max="17" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="13.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="18.5" style="2" customWidth="1"/>
+    <col min="18" max="18" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="P1" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="Q1" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>0.5</v>
       </c>
-      <c r="E2" s="13">
+      <c r="F2" s="13">
         <v>0.05</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="13">
+      <c r="H2" s="13">
         <v>0.05</v>
       </c>
-      <c r="H2" s="15">
+      <c r="I2" s="15">
         <v>1</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>100</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="L2" s="2">
-        <v>100</v>
       </c>
       <c r="M2" s="2">
         <v>100</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="2">
+        <v>100</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="23" t="s">
+      <c r="P2" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="P2" s="23" t="s">
+      <c r="Q2" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="13">
+      <c r="F3" s="13">
         <v>0.05</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="13">
+      <c r="H3" s="13">
         <v>0.05</v>
       </c>
-      <c r="H3" s="15">
+      <c r="I3" s="15">
         <v>1</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>200</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>200</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>100</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="P3" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="R3" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="R3"/>
       <c r="S3"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T3"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="13">
+      <c r="F4" s="13">
         <v>0.05</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>0</v>
       </c>
-      <c r="G4" s="13">
+      <c r="H4" s="13">
         <v>0.05</v>
       </c>
-      <c r="H4" s="15">
+      <c r="I4" s="15">
         <v>1</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>300</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <v>300</v>
       </c>
-      <c r="M4" s="2">
+      <c r="N4" s="2">
         <v>100</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="23" t="s">
+      <c r="P4" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="P4" s="23" t="s">
+      <c r="Q4" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>4</v>
       </c>
-      <c r="E5" s="13">
+      <c r="F5" s="13">
         <v>0.05</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>0</v>
       </c>
-      <c r="G5" s="13">
+      <c r="H5" s="13">
         <v>0.05</v>
       </c>
-      <c r="H5" s="15">
+      <c r="I5" s="15">
         <v>1</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>400</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>400</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>100</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="17" t="s">
+      <c r="P5" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>8</v>
       </c>
-      <c r="E6" s="13">
+      <c r="F6" s="13">
         <v>0.05</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>0</v>
       </c>
-      <c r="G6" s="13">
+      <c r="H6" s="13">
         <v>0.05</v>
       </c>
-      <c r="H6" s="15">
+      <c r="I6" s="15">
         <v>1</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>500</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>500</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <v>100</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="23" t="s">
+      <c r="P6" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="P6" s="23" t="s">
+      <c r="Q6" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="R6" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>16</v>
       </c>
-      <c r="E7" s="13">
+      <c r="F7" s="13">
         <v>0.05</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>0</v>
       </c>
-      <c r="G7" s="13">
+      <c r="H7" s="13">
         <v>0.05</v>
       </c>
-      <c r="H7" s="15">
+      <c r="I7" s="15">
         <v>1</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>500</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>500</v>
       </c>
-      <c r="M7" s="2">
+      <c r="N7" s="2">
         <v>100</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="17" t="s">
+      <c r="P7" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>32</v>
       </c>
-      <c r="E8" s="13">
+      <c r="F8" s="13">
         <v>0.05</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>0</v>
       </c>
-      <c r="G8" s="13">
+      <c r="H8" s="13">
         <v>0.05</v>
       </c>
-      <c r="H8" s="15">
+      <c r="I8" s="15">
         <v>1</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>600</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>600</v>
       </c>
-      <c r="M8" s="2">
+      <c r="N8" s="2">
         <v>100</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="23" t="s">
+      <c r="P8" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="P8" s="23" t="s">
+      <c r="Q8" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>64</v>
       </c>
-      <c r="E9" s="13">
+      <c r="F9" s="13">
         <v>0.05</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>0</v>
       </c>
-      <c r="G9" s="13">
+      <c r="H9" s="13">
         <v>0.05</v>
       </c>
-      <c r="H9" s="15">
+      <c r="I9" s="15">
         <v>1</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>700</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>700</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>100</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="17" t="s">
+      <c r="P9" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="Q9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="R9" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>128</v>
       </c>
-      <c r="E10" s="13">
+      <c r="F10" s="13">
         <v>0.05</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>0</v>
       </c>
-      <c r="G10" s="13">
+      <c r="H10" s="13">
         <v>0.05</v>
       </c>
-      <c r="H10" s="15">
+      <c r="I10" s="15">
         <v>1</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>800</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>800</v>
       </c>
-      <c r="M10" s="2">
+      <c r="N10" s="2">
         <v>100</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23" t="s">
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="R10" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>128</v>
       </c>
-      <c r="E11" s="13">
+      <c r="F11" s="13">
         <v>0.05</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>0</v>
       </c>
-      <c r="G11" s="13">
+      <c r="H11" s="13">
         <v>0.05</v>
       </c>
-      <c r="H11" s="15">
+      <c r="I11" s="15">
         <v>1</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>900</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>900</v>
       </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <v>100</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="O11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="Q11" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="Q11" s="18" t="s">
+      <c r="R11" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="O12" s="23"/>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="P12" s="23"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="O13" s="17"/>
+      <c r="Q12" s="23"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="P13" s="17"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="O14" s="23"/>
+      <c r="Q13" s="17"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="P14" s="23"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="O15" s="17"/>
+      <c r="Q14" s="23"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="P15" s="17"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="O16" s="23"/>
+      <c r="Q15" s="17"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="P16" s="23"/>
-    </row>
-    <row r="17" spans="15:16" x14ac:dyDescent="0.2">
-      <c r="O17" s="17"/>
+      <c r="Q16" s="23"/>
+    </row>
+    <row r="17" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P17" s="17"/>
-    </row>
-    <row r="18" spans="15:16" x14ac:dyDescent="0.2">
-      <c r="O18" s="23"/>
+      <c r="Q17" s="17"/>
+    </row>
+    <row r="18" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P18" s="23"/>
-    </row>
-    <row r="19" spans="15:16" x14ac:dyDescent="0.2">
-      <c r="O19" s="17"/>
+      <c r="Q18" s="23"/>
+    </row>
+    <row r="19" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P19" s="17"/>
-    </row>
-    <row r="20" spans="15:16" x14ac:dyDescent="0.2">
-      <c r="O20" s="23"/>
+      <c r="Q19" s="17"/>
+    </row>
+    <row r="20" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P20" s="23"/>
-    </row>
-    <row r="21" spans="15:16" x14ac:dyDescent="0.2">
-      <c r="O21" s="17"/>
+      <c r="Q20" s="23"/>
+    </row>
+    <row r="21" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2166,54 +2239,60 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$C$2:$C$17</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C300</xm:sqref>
+          <xm:sqref>D2:D300</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$N$2:$N$4</xm:f>
           </x14:formula1>
-          <xm:sqref>R3</xm:sqref>
+          <xm:sqref>S3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$O$2:$O$3</xm:f>
           </x14:formula1>
-          <xm:sqref>S3</xm:sqref>
+          <xm:sqref>T3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$Q$2:$Q$5</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:N300 O22:O300</xm:sqref>
+          <xm:sqref>O2:O300</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$S$2:$S$11</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:Q1048576</xm:sqref>
+          <xm:sqref>R2:R1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$I$2:$I$6</xm:f>
           </x14:formula1>
-          <xm:sqref>J1:J1048576</xm:sqref>
+          <xm:sqref>K1:K1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Help!$T$2:$T$5</xm:f>
+            <xm:f>Help!$U$2:$U$5</xm:f>
           </x14:formula1>
-          <xm:sqref>P1:P1048576</xm:sqref>
+          <xm:sqref>Q1:Q1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$T$2:$T$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>P2:P1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2223,10 +2302,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T28"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2250,11 +2329,12 @@
     <col min="17" max="17" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.83203125" style="2"/>
+    <col min="20" max="20" width="26.6640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2312,11 +2392,14 @@
       <c r="S1" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="24" t="s">
+      <c r="T1" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="U1" s="24" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -2374,11 +2457,14 @@
       <c r="S2" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="U2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>41</v>
       </c>
@@ -2427,11 +2513,14 @@
       <c r="S3" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="U3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>44</v>
       </c>
@@ -2456,11 +2545,12 @@
       <c r="S4" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="19"/>
+      <c r="U4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
@@ -2479,11 +2569,11 @@
       <c r="S5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>55</v>
       </c>
@@ -2496,16 +2586,18 @@
       <c r="S6" s="19" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T6" s="19"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>56</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
         <v>57</v>
       </c>
@@ -2515,7 +2607,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
         <v>58</v>
       </c>
@@ -2524,8 +2616,9 @@
       <c r="S9" s="20" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T9" s="20"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
         <v>59</v>
       </c>
@@ -2535,7 +2628,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="s">
         <v>60</v>
       </c>
@@ -2544,36 +2637,37 @@
       <c r="S11" s="20" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T11" s="20"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
         <v>61</v>
       </c>
       <c r="Q12"/>
       <c r="R12"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
         <v>62</v>
       </c>
       <c r="Q13"/>
       <c r="R13"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
         <v>63</v>
       </c>
       <c r="Q14"/>
       <c r="R14"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
         <v>64</v>
       </c>
       <c r="Q15"/>
       <c r="R15"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
added new column: burstable instances
</commit_message>
<xml_diff>
--- a/input_generic.xlsx
+++ b/input_generic.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="86">
   <si>
     <t>Description</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>Cold HDD</t>
+  </si>
+  <si>
+    <t>Use Burstable Performance</t>
+  </si>
+  <si>
+    <t>Server 2</t>
   </si>
 </sst>
 </file>
@@ -301,6 +307,7 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -323,12 +330,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -336,11 +345,13 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -354,6 +365,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -361,6 +373,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -479,7 +492,7 @@
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="42">
     <dxf>
       <font>
         <b val="0"/>
@@ -851,6 +864,24 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1225,25 +1256,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:R1048576" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
-  <autoFilter ref="A1:R1048576"/>
-  <tableColumns count="18">
-    <tableColumn id="1" name="Description" dataDxfId="38"/>
-    <tableColumn id="14" name="Instances" dataDxfId="37"/>
-    <tableColumn id="2" name="Environment" dataDxfId="36"/>
-    <tableColumn id="3" name="Region" dataDxfId="35"/>
-    <tableColumn id="4" name="CPU" dataDxfId="34"/>
-    <tableColumn id="6" name="CPU Tolerance" dataDxfId="33" dataCellStyle="Percent"/>
-    <tableColumn id="17" name="Memory" dataDxfId="32"/>
-    <tableColumn id="7" name="Memory Tolerance" dataDxfId="31" dataCellStyle="Percent"/>
-    <tableColumn id="8" name="Monthly Utilization" dataDxfId="30"/>
-    <tableColumn id="9" name="Storage(GB)" dataDxfId="29"/>
-    <tableColumn id="10" name="Volume Type" dataDxfId="28"/>
-    <tableColumn id="11" name="IOPS" dataDxfId="27"/>
-    <tableColumn id="12" name="Snapshot(GB)" dataDxfId="26"/>
-    <tableColumn id="21" name="S3 Backup(GB)" dataDxfId="25"/>
-    <tableColumn id="18" name="Operating System" dataDxfId="24"/>
-    <tableColumn id="13" name="Only Current Generation Instances" dataDxfId="23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S1048576" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="A1:S1048576"/>
+  <tableColumns count="19">
+    <tableColumn id="1" name="Description" dataDxfId="39"/>
+    <tableColumn id="14" name="Instances" dataDxfId="38"/>
+    <tableColumn id="2" name="Environment" dataDxfId="37"/>
+    <tableColumn id="3" name="Region" dataDxfId="36"/>
+    <tableColumn id="4" name="CPU" dataDxfId="35"/>
+    <tableColumn id="6" name="CPU Tolerance" dataDxfId="34" dataCellStyle="Percent"/>
+    <tableColumn id="17" name="Memory" dataDxfId="33"/>
+    <tableColumn id="7" name="Memory Tolerance" dataDxfId="32" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="Monthly Utilization" dataDxfId="31"/>
+    <tableColumn id="9" name="Storage(GB)" dataDxfId="30"/>
+    <tableColumn id="10" name="Volume Type" dataDxfId="29"/>
+    <tableColumn id="11" name="IOPS" dataDxfId="28"/>
+    <tableColumn id="12" name="Snapshot(GB)" dataDxfId="27"/>
+    <tableColumn id="21" name="S3 Backup(GB)" dataDxfId="26"/>
+    <tableColumn id="18" name="Operating System" dataDxfId="25"/>
+    <tableColumn id="13" name="Only Current Generation Instances" dataDxfId="24"/>
+    <tableColumn id="15" name="Use Burstable Performance" dataDxfId="23"/>
     <tableColumn id="5" name="Pre Installed S/W" dataDxfId="22"/>
     <tableColumn id="22" name="Billing Option" dataDxfId="21"/>
   </tableColumns>
@@ -1553,18 +1585,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:R11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
@@ -1576,12 +1608,14 @@
     <col min="13" max="13" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="18.5" style="2" customWidth="1"/>
-    <col min="18" max="18" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.83203125" style="2"/>
+    <col min="16" max="16" width="32.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1631,89 +1665,187 @@
         <v>78</v>
       </c>
       <c r="Q1" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="R1" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="P3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3"/>
-      <c r="T3"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="I2" s="15">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="R2" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="I3" s="15">
+        <v>1</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q3" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="R3" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P4" s="23"/>
       <c r="Q4" s="23"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R4" s="23"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P5" s="17"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q5" s="17"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P6" s="23"/>
       <c r="Q6" s="23"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R6" s="23"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P7" s="17"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q7" s="17"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P8" s="23"/>
       <c r="Q8" s="23"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R8" s="23"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P9" s="17"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q9" s="17"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P10" s="23"/>
       <c r="Q10" s="23"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="R11" s="18"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R10" s="23"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S11" s="18"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P12" s="23"/>
       <c r="Q12" s="23"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R12" s="23"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P13" s="17"/>
       <c r="Q13" s="17"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R13" s="17"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P14" s="23"/>
       <c r="Q14" s="23"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R14" s="23"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P15" s="17"/>
       <c r="Q15" s="17"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R15" s="17"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P16" s="23"/>
       <c r="Q16" s="23"/>
-    </row>
-    <row r="17" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="R16" s="23"/>
+    </row>
+    <row r="17" spans="16:18" x14ac:dyDescent="0.2">
       <c r="P17" s="17"/>
       <c r="Q17" s="17"/>
-    </row>
-    <row r="18" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="R17" s="17"/>
+    </row>
+    <row r="18" spans="16:18" x14ac:dyDescent="0.2">
       <c r="P18" s="23"/>
       <c r="Q18" s="23"/>
-    </row>
-    <row r="19" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="R18" s="23"/>
+    </row>
+    <row r="19" spans="16:18" x14ac:dyDescent="0.2">
       <c r="P19" s="17"/>
       <c r="Q19" s="17"/>
-    </row>
-    <row r="20" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="R19" s="17"/>
+    </row>
+    <row r="20" spans="16:18" x14ac:dyDescent="0.2">
       <c r="P20" s="23"/>
       <c r="Q20" s="23"/>
-    </row>
-    <row r="21" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="R20" s="23"/>
+    </row>
+    <row r="21" spans="16:18" x14ac:dyDescent="0.2">
       <c r="P21" s="17"/>
       <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1723,24 +1855,12 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$C$2:$C$17</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D300</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Help!$N$2:$N$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>S3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Help!$O$2:$O$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>T3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -1758,7 +1878,7 @@
           <x14:formula1>
             <xm:f>Help!$S$2:$S$11</xm:f>
           </x14:formula1>
-          <xm:sqref>R2:R1048576</xm:sqref>
+          <xm:sqref>S2:S1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -1770,13 +1890,13 @@
           <x14:formula1>
             <xm:f>Help!$U$2:$U$5</xm:f>
           </x14:formula1>
-          <xm:sqref>Q1:Q1048576</xm:sqref>
+          <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$T$2:$T$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P1048576</xm:sqref>
+          <xm:sqref>P2:Q1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updated Memory column name
Updated Memory column name and number format in multiple columns
</commit_message>
<xml_diff>
--- a/input_generic.xlsx
+++ b/input_generic.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Servers" sheetId="1" r:id="rId1"/>
     <sheet name="Help" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="94">
   <si>
     <t>Description</t>
   </si>
@@ -289,6 +289,27 @@
   </si>
   <si>
     <t>Server 3</t>
+  </si>
+  <si>
+    <t>Server 4</t>
+  </si>
+  <si>
+    <t>Server 5</t>
+  </si>
+  <si>
+    <t>Server 6</t>
+  </si>
+  <si>
+    <t>Server 7</t>
+  </si>
+  <si>
+    <t>Server 8</t>
+  </si>
+  <si>
+    <t>Server 9</t>
+  </si>
+  <si>
+    <t>Memory(GB)</t>
   </si>
 </sst>
 </file>
@@ -448,7 +469,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -467,9 +488,6 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -477,7 +495,9 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -975,6 +995,60 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -993,6 +1067,114 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1029,169 +1211,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1260,8 +1280,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S1048576" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
-  <autoFilter ref="A1:S1048576"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S1048565" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="A1:S1048565"/>
   <tableColumns count="19">
     <tableColumn id="1" name="Description" dataDxfId="39"/>
     <tableColumn id="14" name="Instances" dataDxfId="38"/>
@@ -1269,14 +1289,20 @@
     <tableColumn id="3" name="Region" dataDxfId="36"/>
     <tableColumn id="4" name="CPU" dataDxfId="35"/>
     <tableColumn id="6" name="CPU Tolerance" dataDxfId="34" dataCellStyle="Percent"/>
-    <tableColumn id="17" name="Memory" dataDxfId="33"/>
+    <tableColumn id="17" name="Memory(GB)" dataDxfId="33"/>
     <tableColumn id="7" name="Memory Tolerance" dataDxfId="32" dataCellStyle="Percent"/>
     <tableColumn id="8" name="Monthly Utilization" dataDxfId="31"/>
     <tableColumn id="9" name="Storage(GB)" dataDxfId="30"/>
-    <tableColumn id="10" name="Volume Type" dataDxfId="29"/>
+    <tableColumn id="10" name="Volume Type" dataDxfId="29">
+      <calculatedColumnFormula>IF(J2&lt;50,"Magnetic","General Purpose")</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="11" name="IOPS" dataDxfId="28"/>
-    <tableColumn id="12" name="Snapshot(GB)" dataDxfId="27"/>
-    <tableColumn id="21" name="S3 Backup(GB)" dataDxfId="26"/>
+    <tableColumn id="12" name="Snapshot(GB)" dataDxfId="27">
+      <calculatedColumnFormula>(J2*1.5)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="21" name="S3 Backup(GB)" dataDxfId="26">
+      <calculatedColumnFormula>(G2*2)</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="18" name="Operating System" dataDxfId="25"/>
     <tableColumn id="13" name="Only Current Generation Instances" dataDxfId="24"/>
     <tableColumn id="15" name="Use Burstable Performance" dataDxfId="23"/>
@@ -1589,28 +1615,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" style="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.83203125" style="15" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" style="25" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" style="25" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.5" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="32.5" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="26.5" style="2" bestFit="1" customWidth="1"/>
@@ -1639,7 +1665,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>5</v>
@@ -1665,13 +1691,13 @@
       <c r="O1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="Q1" s="22" t="s">
+      <c r="Q1" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="R1" s="21" t="s">
         <v>73</v>
       </c>
       <c r="S1" s="6" t="s">
@@ -1682,7 +1708,7 @@
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="25">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1691,31 +1717,43 @@
       <c r="D2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="25">
         <v>1</v>
       </c>
       <c r="F2" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="G2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" s="27">
         <v>1</v>
       </c>
       <c r="H2" s="13">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="I2" s="15">
         <v>1</v>
       </c>
+      <c r="J2" s="25">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" s="25">
+        <v>15</v>
+      </c>
+      <c r="N2" s="25">
+        <v>2</v>
+      </c>
       <c r="O2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="Q2" s="23" t="s">
+      <c r="Q2" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="R2" s="23" t="s">
+      <c r="R2" s="22" t="s">
         <v>74</v>
       </c>
       <c r="S2" s="2" t="s">
@@ -1726,7 +1764,7 @@
       <c r="A3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="25">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1735,29 +1773,41 @@
       <c r="D3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="25">
         <v>1</v>
       </c>
       <c r="F3" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="27">
+        <v>2</v>
       </c>
       <c r="H3" s="13">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="I3" s="15">
         <v>1</v>
       </c>
+      <c r="J3" s="25">
+        <v>45</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="25">
+        <v>67.5</v>
+      </c>
+      <c r="N3" s="25">
+        <v>2</v>
+      </c>
       <c r="O3" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="P3" s="26" t="s">
         <v>80</v>
       </c>
       <c r="Q3" s="26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="R3" s="26" t="s">
         <v>74</v>
@@ -1770,7 +1820,7 @@
       <c r="A4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="25">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1779,14 +1829,14 @@
       <c r="D4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="25">
         <v>4</v>
       </c>
       <c r="F4" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="G4" s="2">
-        <v>8</v>
+        <v>0.1</v>
+      </c>
+      <c r="G4" s="27">
+        <v>4</v>
       </c>
       <c r="H4" s="13">
         <v>0.1</v>
@@ -1794,114 +1844,360 @@
       <c r="I4" s="15">
         <v>1</v>
       </c>
-      <c r="J4" s="2">
-        <v>22</v>
+      <c r="J4" s="25">
+        <v>100</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="2">
-        <v>20</v>
+      <c r="M4" s="25">
+        <v>150</v>
+      </c>
+      <c r="N4" s="25">
+        <v>8</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="Q4" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="R4" s="23" t="s">
-        <v>74</v>
-      </c>
+      <c r="Q4" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="R4" s="22"/>
       <c r="S4" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
+      <c r="A5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="25">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="25">
+        <v>4</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="G5" s="27">
+        <v>16</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I5" s="15">
+        <v>1</v>
+      </c>
+      <c r="J5" s="25">
+        <v>20</v>
+      </c>
+      <c r="K5" s="2" t="str">
+        <f>IF(J5&lt;50,"Magnetic","General Purpose")</f>
+        <v>Magnetic</v>
+      </c>
+      <c r="M5" s="25">
+        <v>30</v>
+      </c>
+      <c r="N5" s="25">
+        <v>32</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
+      <c r="A6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="25">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="25">
+        <v>4</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="27">
+        <v>7</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I6" s="15">
+        <v>1</v>
+      </c>
+      <c r="J6" s="25">
+        <v>45</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M6" s="25">
+        <v>67.5</v>
+      </c>
+      <c r="N6" s="25">
+        <v>14</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q6" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="R6" s="22"/>
+      <c r="S6" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
+      <c r="A7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="25">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="25">
+        <v>4</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="27">
+        <v>7</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="15">
+        <v>1</v>
+      </c>
+      <c r="J7" s="25">
+        <v>40</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M7" s="25">
+        <v>60</v>
+      </c>
+      <c r="N7" s="25">
+        <v>14</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q7" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
+      <c r="A8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="25">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="25">
+        <v>4</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="G8" s="27">
+        <v>15</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I8" s="15">
+        <v>1</v>
+      </c>
+      <c r="J8" s="25">
+        <v>100</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="25">
+        <v>150</v>
+      </c>
+      <c r="N8" s="25">
+        <v>30</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q8" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="R8" s="22"/>
+      <c r="S8" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
+      <c r="A9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="25">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="25">
+        <v>4</v>
+      </c>
+      <c r="F9" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="G9" s="27">
+        <v>32</v>
+      </c>
+      <c r="H9" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I9" s="15">
+        <v>1</v>
+      </c>
+      <c r="J9" s="25">
+        <v>150</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="25">
+        <v>225</v>
+      </c>
+      <c r="N9" s="25">
+        <v>64</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q9" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="S11" s="18"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-    </row>
-    <row r="17" spans="16:18" x14ac:dyDescent="0.2">
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-    </row>
-    <row r="18" spans="16:18" x14ac:dyDescent="0.2">
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-    </row>
-    <row r="19" spans="16:18" x14ac:dyDescent="0.2">
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-    </row>
-    <row r="20" spans="16:18" x14ac:dyDescent="0.2">
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
-    </row>
-    <row r="21" spans="16:18" x14ac:dyDescent="0.2">
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
+      <c r="A10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="25">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="25">
+        <v>4</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="G10" s="27">
+        <v>16</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="15">
+        <v>1</v>
+      </c>
+      <c r="J10" s="25">
+        <v>30</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M10" s="25">
+        <v>45</v>
+      </c>
+      <c r="N10" s="25">
+        <v>32</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q10" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="R10" s="22"/>
+      <c r="S10" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="K2:K4 K6:K10 N2:N10 M2:M10" calculatedColumn="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -1912,43 +2208,43 @@
           <x14:formula1>
             <xm:f>Help!$C$2:$C$17</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D300</xm:sqref>
+          <xm:sqref>D2:D289</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$Q$2:$Q$5</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O300</xm:sqref>
+          <xm:sqref>O2:O289</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
+          <xm:sqref>C2:C1048565</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$S$2:$S$11</xm:f>
           </x14:formula1>
-          <xm:sqref>S2:S1048576</xm:sqref>
+          <xm:sqref>S2:S1048565</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$I$2:$I$6</xm:f>
           </x14:formula1>
-          <xm:sqref>K1:K1048576</xm:sqref>
+          <xm:sqref>K1:K1048565</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$U$2:$U$5</xm:f>
           </x14:formula1>
-          <xm:sqref>R1:R1048576</xm:sqref>
+          <xm:sqref>R1:R1048565</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$T$2:$T$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:Q1048576</xm:sqref>
+          <xm:sqref>P2:Q1048565</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2045,13 +2341,13 @@
       <c r="R1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="T1" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="U1" s="24" t="s">
+      <c r="U1" s="23" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2110,10 +2406,10 @@
       <c r="R2" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="19" t="s">
+      <c r="S2" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="T2" s="19" t="s">
+      <c r="T2" s="18" t="s">
         <v>80</v>
       </c>
       <c r="U2" t="s">
@@ -2166,10 +2462,10 @@
       <c r="R3" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="20" t="s">
+      <c r="S3" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="T3" s="20" t="s">
+      <c r="T3" s="19" t="s">
         <v>79</v>
       </c>
       <c r="U3" t="s">
@@ -2198,10 +2494,10 @@
       <c r="R4" t="s">
         <v>49</v>
       </c>
-      <c r="S4" s="19" t="s">
+      <c r="S4" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="T4" s="19"/>
+      <c r="T4" s="18"/>
       <c r="U4" t="s">
         <v>76</v>
       </c>
@@ -2239,10 +2535,10 @@
       <c r="I6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="S6" s="19" t="s">
+      <c r="S6" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="T6" s="19"/>
+      <c r="T6" s="18"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
@@ -2269,10 +2565,10 @@
       </c>
       <c r="Q9"/>
       <c r="R9"/>
-      <c r="S9" s="20" t="s">
+      <c r="S9" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="T9" s="20"/>
+      <c r="T9" s="19"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
@@ -2290,10 +2586,10 @@
       </c>
       <c r="Q11"/>
       <c r="R11"/>
-      <c r="S11" s="20" t="s">
+      <c r="S11" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="T11" s="20"/>
+      <c r="T11" s="19"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">

</xml_diff>

<commit_message>
R5 and Bare Metal
</commit_message>
<xml_diff>
--- a/input_generic.xlsx
+++ b/input_generic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravanini/WorkDocs/workspace/ProposalCalculator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carvaa/Documents/GitHub/ProposalCalculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67E44439-2CAA-CA47-B069-27A61EDC074D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B0D02840-82C8-C049-826A-C773D7B030AC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Servers" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="94">
   <si>
     <t>Description</t>
   </si>
@@ -1618,8 +1618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1716,7 +1716,7 @@
         <v>39</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="E2" s="25">
         <v>1</v>
@@ -1737,10 +1737,10 @@
         <v>10</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="M2" s="25">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N2" s="25">
         <v>2</v>
@@ -1772,7 +1772,7 @@
         <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="E3" s="25">
         <v>1</v>
@@ -1790,13 +1790,13 @@
         <v>1</v>
       </c>
       <c r="J3" s="25">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="M3" s="25">
-        <v>67.5</v>
+        <v>10</v>
       </c>
       <c r="N3" s="25">
         <v>2</v>
@@ -1828,7 +1828,7 @@
         <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E4" s="25">
         <v>4</v>
@@ -1846,13 +1846,13 @@
         <v>1</v>
       </c>
       <c r="J4" s="25">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>34</v>
       </c>
       <c r="M4" s="25">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="N4" s="25">
         <v>8</v>
@@ -1866,7 +1866,9 @@
       <c r="Q4" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="R4" s="22"/>
+      <c r="R4" s="26" t="s">
+        <v>74</v>
+      </c>
       <c r="S4" s="2" t="s">
         <v>63</v>
       </c>
@@ -1882,7 +1884,7 @@
         <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="E5" s="25">
         <v>4</v>
@@ -1900,14 +1902,13 @@
         <v>1</v>
       </c>
       <c r="J5" s="25">
-        <v>20</v>
-      </c>
-      <c r="K5" s="2" t="str">
-        <f>IF(J5&lt;50,"Magnetic","General Purpose")</f>
-        <v>Magnetic</v>
+        <v>10</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="M5" s="25">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="N5" s="25">
         <v>32</v>
@@ -1920,6 +1921,9 @@
       </c>
       <c r="Q5" s="26" t="s">
         <v>80</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>74</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>63</v>
@@ -1954,13 +1958,13 @@
         <v>1</v>
       </c>
       <c r="J6" s="25">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="M6" s="25">
-        <v>67.5</v>
+        <v>10</v>
       </c>
       <c r="N6" s="25">
         <v>14</v>
@@ -1974,7 +1978,9 @@
       <c r="Q6" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="R6" s="22"/>
+      <c r="R6" s="26" t="s">
+        <v>74</v>
+      </c>
       <c r="S6" s="2" t="s">
         <v>63</v>
       </c>
@@ -1990,7 +1996,7 @@
         <v>37</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="E7" s="25">
         <v>4</v>
@@ -2008,13 +2014,13 @@
         <v>1</v>
       </c>
       <c r="J7" s="25">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="M7" s="25">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="N7" s="25">
         <v>14</v>
@@ -2027,6 +2033,9 @@
       </c>
       <c r="Q7" s="26" t="s">
         <v>80</v>
+      </c>
+      <c r="R7" s="26" t="s">
+        <v>74</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>63</v>
@@ -2043,7 +2052,7 @@
         <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E8" s="25">
         <v>4</v>
@@ -2061,13 +2070,13 @@
         <v>1</v>
       </c>
       <c r="J8" s="25">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="M8" s="25">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="N8" s="25">
         <v>30</v>
@@ -2081,7 +2090,9 @@
       <c r="Q8" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="R8" s="22"/>
+      <c r="R8" s="26" t="s">
+        <v>74</v>
+      </c>
       <c r="S8" s="2" t="s">
         <v>63</v>
       </c>
@@ -2097,7 +2108,7 @@
         <v>40</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="E9" s="25">
         <v>4</v>
@@ -2115,13 +2126,13 @@
         <v>1</v>
       </c>
       <c r="J9" s="25">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>34</v>
       </c>
       <c r="M9" s="25">
-        <v>225</v>
+        <v>10</v>
       </c>
       <c r="N9" s="25">
         <v>64</v>
@@ -2134,6 +2145,9 @@
       </c>
       <c r="Q9" s="26" t="s">
         <v>79</v>
+      </c>
+      <c r="R9" s="26" t="s">
+        <v>74</v>
       </c>
       <c r="S9" s="2" t="s">
         <v>63</v>
@@ -2150,7 +2164,7 @@
         <v>39</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="E10" s="25">
         <v>4</v>
@@ -2168,13 +2182,13 @@
         <v>1</v>
       </c>
       <c r="J10" s="25">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="M10" s="25">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="N10" s="25">
         <v>32</v>
@@ -2188,7 +2202,9 @@
       <c r="Q10" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="R10" s="22"/>
+      <c r="R10" s="26" t="s">
+        <v>74</v>
+      </c>
       <c r="S10" s="2" t="s">
         <v>63</v>
       </c>
@@ -2197,7 +2213,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="K2:K4 K6:K10 N2:N10 M2:M10" calculatedColumn="1"/>
+    <ignoredError sqref="N2:N10" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>